<commit_message>
Updated USA model - 2025-07-29 09:38
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_USA/SuppXLS/Scen_Base_VS.xlsx
@@ -20,7 +20,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -51,8 +51,11 @@
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
@@ -71,6 +74,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DCE6F1"/>
+        <bgColor rgb="00DCE6F1"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -85,7 +94,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="1" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -98,6 +107,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -542,27 +552,27 @@
       </c>
     </row>
     <row r="2">
-      <c r="F2" t="inlineStr">
+      <c r="F2" s="10" t="inlineStr">
         <is>
           <t>model_fuel</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="G2" s="10" t="inlineStr">
         <is>
           <t>ember_min</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="H2" s="10" t="inlineStr">
         <is>
           <t>ember_max</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="I2" s="10" t="inlineStr">
         <is>
           <t>irena_min</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
+      <c r="J2" s="10" t="inlineStr">
         <is>
           <t>irena_max</t>
         </is>
@@ -579,17 +589,17 @@
           <t>bioenergy</t>
         </is>
       </c>
-      <c r="G3" t="n">
-        <v>0.5486</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.8905999999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.5787</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.9437</v>
+      <c r="G3" s="7" t="n">
+        <v>0.548630471262293</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0.8906252231919665</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>0.5786929779210424</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>0.9436581186830296</v>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
@@ -634,17 +644,17 @@
           <t>coal</t>
         </is>
       </c>
-      <c r="G4" t="n">
-        <v>0.3788</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.6899</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.4513</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.7824</v>
+      <c r="G4" s="7" t="n">
+        <v>0.3788471064210663</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0.6899337540969159</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>0.4512847106507687</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>0.7823690317958011</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -686,17 +696,17 @@
           <t>gas</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>0.2325</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.4346</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.2145</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.3947</v>
+      <c r="G5" s="7" t="n">
+        <v>0.2325433778504463</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0.4345941432434282</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>0.2145271387405906</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>0.3946615645986714</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -741,17 +751,17 @@
           <t>geothermal</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="7" t="n">
         <v/>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="7" t="n">
         <v/>
       </c>
-      <c r="I6" t="n">
-        <v>0.5976</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.8767</v>
+      <c r="I6" s="7" t="n">
+        <v>0.5975882301971498</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>0.8767485700120137</v>
       </c>
       <c r="U6" t="inlineStr">
         <is>
@@ -784,17 +794,17 @@
           <t>hydro</t>
         </is>
       </c>
-      <c r="G7" t="n">
-        <v>0.3011</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.4333</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.2487</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.3893</v>
+      <c r="G7" s="7" t="n">
+        <v>0.3010678405043429</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0.4332638294690846</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>0.2486541769844115</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>0.3892785813467925</v>
       </c>
       <c r="U7" t="inlineStr">
         <is>
@@ -886,17 +896,17 @@
           <t>nuclear</t>
         </is>
       </c>
-      <c r="G8" t="n">
-        <v>0.8619</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.9417</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.8976</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9812</v>
+      <c r="G8" s="7" t="n">
+        <v>0.8619399289501483</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0.9416877479258461</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>0.8976108572584858</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>0.9811611201215411</v>
       </c>
       <c r="U8" t="inlineStr">
         <is>
@@ -957,17 +967,17 @@
           <t>oil</t>
         </is>
       </c>
-      <c r="G9" t="n">
-        <v>0.0885</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.2424</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0.1121</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.2911</v>
+      <c r="G9" s="7" t="n">
+        <v>0.08850048303779549</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0.2424212560213349</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>0.1121355917983518</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>0.2910793279594932</v>
       </c>
       <c r="U9" t="inlineStr">
         <is>
@@ -1031,17 +1041,17 @@
           <t>solar</t>
         </is>
       </c>
-      <c r="G10" t="n">
-        <v>0.0368</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.205</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0.1257</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0.1871</v>
+      <c r="G10" s="7" t="n">
+        <v>0.03683733281518184</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0.2049920032039881</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>0.1257154045972798</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>0.1870506479609498</v>
       </c>
     </row>
     <row r="11" ht="14.65" customHeight="1">
@@ -1050,17 +1060,17 @@
           <t>wind</t>
         </is>
       </c>
-      <c r="G11" t="n">
-        <v>0.1993</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.35</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0.2011</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.3539</v>
+      <c r="G11" s="7" t="n">
+        <v>0.1993280810088248</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <v>0.349951475758991</v>
+      </c>
+      <c r="I11" s="7" t="n">
+        <v>0.2010903291376542</v>
+      </c>
+      <c r="J11" s="7" t="n">
+        <v>0.3539464426516985</v>
       </c>
     </row>
     <row r="13">

</xml_diff>